<commit_message>
Added Abhidharma Aruth Desana on Aug 15th
</commit_message>
<xml_diff>
--- a/working/a151notes.xlsx
+++ b/working/a151notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/374644a6aeffffba/Teaching/2024 Spring/Home/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="11_F25DC773A252ABDACC1048E881D96D985ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F07CF24B-26B0-4883-AA14-B9828DCF1866}"/>
+  <xr:revisionPtr revIDLastSave="315" documentId="11_F25DC773A252ABDACC1048E881D96D985ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D14493C9-225B-4BA4-BFB4-14A08B252BE2}"/>
   <bookViews>
-    <workbookView xWindow="27615" yWindow="3735" windowWidth="22950" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18105" yWindow="3240" windowWidth="22950" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="133">
   <si>
     <t>ප්‍රත්‍ය</t>
   </si>
@@ -1224,17 +1224,390 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>දේහේතුක, ත්‍රිහේතුකs cjk</t>
+    <t>චිත්තජ රූප, හාර්දය වස්තුවෙන් අන්‍ය වූ ප්‍රතිසන්ධී කර්මජ රූප, සකල උපාදාය රූප</t>
+  </si>
+  <si>
+    <t>නැත</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">සිත් 89, චෛතසික </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>52</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Iskoola Pota"/>
+        <family val="2"/>
+      </rPr>
+      <t>,  සකල මහා භූතයෝ, ප්‍රතිසන්ධි වස්තු රූප</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">සිත් 89, චෛතසික </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>52</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>සිත් 89</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Iskoola Pota"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> චෛතසික 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Iskoola Pota"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, රූප </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>28</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Iskoola Pota"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, නිර්වාණය, ප්‍රඥප්තින් </t>
+    </r>
+  </si>
+  <si>
+    <t>සිත් 89 හි ඇති චේතනාව</t>
+  </si>
+  <si>
+    <t>අතීත වූ කුසල අකුසල චේතනා 33</t>
+  </si>
+  <si>
+    <t>විපාක ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>විපාක සිත් 36, චෛතසික 38, යන ප්‍රවුර්ත්ති ප්‍රතිසන්ධි නාමස්කන්ධ</t>
+  </si>
+  <si>
+    <t>නාම ආහාර ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>රූප ආහාර ප්‍රත්‍යය (උපත්ථමභකත්වය)</t>
+  </si>
+  <si>
+    <t>රූප ආහාර ප්‍රත්‍යය (ජනකත්වය)</t>
+  </si>
+  <si>
+    <t>ඔවුනොවුන්ට හා චිත්තජ රූප ප්‍රතිසන්ධි කර්මජ රුපයන්ට ද ප්‍රත්‍යය ව සිත් 89, චෛතසික 52 යන ප්‍රතිසන්ධි නාමස්කන්ධ,ඔවුනොවුන්ට හා උපාදාය රුපයන්ට ප්‍රත්‍යය වන චිත්තජ ප්‍රතිසන්ධි කර්මජ බාහිර අහාරාජ ඍතුජ අසංඥ සත්ව කර්මජ ප්‍රවුර්තික කර්මජ රූපයන්ට අයත් වූ සකල මහා භූතයෝ ය, පඤවවොකාර  ප්‍රතිසන්ධි නාමස්කන්ධයන්ට ප්‍රත්‍යය වන හර්දය වස්තුව ය, හර්දය වස්තුවට ප්‍රත්‍යය වන පඤවවොකාර ප්‍රතිසන්ධි නාමස්කන්ධ</t>
+  </si>
+  <si>
+    <t>ඔවුනොවුන්ගෙන් ප්‍රත්‍යය ලබන සිත් 89, චෛතසික 52, යන ප්‍රවුර්ත්ති ප්‍රතිසන්ධි නාමස්කන්ධ,  නාමස්කන්ධයන්ගෙන් ප්‍රත්‍යය ලබන චිත්තජ රූප හා ප්‍රතිසන්ධි කර්මජ රූප, ඔවුනොවුන්ගෙන් ප්‍රත්‍යය ලබන සකල මහා  භූතයෝ,  මහා භූතයන්ගෙන් ප්‍රත්‍යය ලබන උපදය රූප, හර්දයවස්තුවෙන් ප්‍රත්‍යය ලබන පඤවෝකාර  ප්‍රතිසන්ධි නාමස්කන්ධ, පඤවෝකාර ප්‍රතිසන්ධි නාමස්කන්ධයන්ගෙන් ප්‍රත්‍යය ලබන හර්දය වස්තුව</t>
+  </si>
+  <si>
+    <t>චිත්තජ රූප, ප්‍රතිසන්ධී කර්මජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඤ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප (රූප සියල්ල)</t>
+  </si>
+  <si>
+    <t>චිත්තජ රූප, ප්‍රතිසන්ධී කර්මජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඤ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප</t>
+  </si>
+  <si>
+    <t>අවිගත ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>විගත ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>නාස්ති  ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">අහේතුක සිත් </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>18,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Iskoola Pota"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ඡන්දය වර්ජිත අන්‍යසමාන චෛතසික </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Iskoola Pota"/>
+        <family val="2"/>
+      </rPr>
+      <t>, මෝහ මූල ද්විත්වයේ (සිත් දෙකේ) මෝහය, අහේතුක චිත්තජ රූප, අහේතුක ප්‍රතිසන්ධි කර්මජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඥ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප</t>
+    </r>
+  </si>
+  <si>
+    <t>සිත් 89, චේතනාව හැර චෛතසික 51, චිත්තජ රූප, ප්‍රතිසන්ධී කර්මජ රූප</t>
+  </si>
+  <si>
+    <t>සිත් 89හි ඇති චේතනා 89, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඥ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප</t>
+  </si>
+  <si>
+    <t>විපාක සිත් 36, අහි ඇතුලත්  චෛතසික 38, චිත්තජ රූප, ප්‍රතිසන්ධී කර්මජ රූප,  අසංඥ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප</t>
+  </si>
+  <si>
+    <t>වර්තමාන</t>
+  </si>
+  <si>
+    <t>සම්පයුත්ත ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>අස්ථි ප්‍රත්‍යයට සමානයි</t>
+  </si>
+  <si>
+    <t>ආරම්මණුපනිස්සය ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>අනන්තරූප නිස්සය ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t xml:space="preserve">පකතූප නිස්සය ප්‍රත්‍යය </t>
+  </si>
+  <si>
+    <t xml:space="preserve">සිත් 89, චෛතසික 52, රූප 28, ඇතැම්  ප්‍රඥප්තින් </t>
+  </si>
+  <si>
+    <t>ප්‍රවුර්ත්ති ප්‍රතිසන්ධි වශයෙන් සකල සිත් 89, චෛතසික 52</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> සමනන්තර ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>අනන්තර ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>සහාජාත ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t xml:space="preserve">සිත් 89, චෛතසික 52, සකල මහා භූතයෝ ය,   ප්‍රතිසන්ධිවස්තු රූප </t>
+  </si>
+  <si>
+    <t>m[apfjdaldr Njfhys my&lt;
+jk wjia:dfjys wrEm úmdl i;r yer ufkda ú[aØK Od;=
+ye;a;Etl h" චෛතසික 52</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">සහාජාත අධිපති ප්‍රත්‍යය නොලබන්නාවූද, සහාජාත අධිපති ප්‍රත්‍යය නොලබන්න අවස්ථාවේ වූද කාමාවචර සිත් </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>54</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Iskoola Pota"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, මහග්ගත විපාක සිත් 9, එහි යෙදන චෛතසික </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>52</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Iskoola Pota"/>
+        <family val="2"/>
+      </rPr>
+      <t>, ඒ ඒ  අවස්ථාව අධිපති ප්‍රත්‍යවන ධර්ම,  නිරාධිපති චිත්තජ රූප, ප්‍රතිසන්ධී කර්මජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඥ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">කුසල් සිත් 21, අකුසල් සිත් 12, ක්‍රියා සිත් 20, චෛතසික 52, චිත්තජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප </t>
+  </si>
+  <si>
+    <t xml:space="preserve">මාර්ග-ඵල ජවන වර්ජිත පූර්ව පූර්ව වූ ලෞකික ජවන 47, චෛතසික </t>
+  </si>
+  <si>
+    <t>ආසෙවන ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t xml:space="preserve">මාර්ග-ඵල ජවන වර්ජිත පශ්විම පශ්විම ජවන් 51, චෛතසික </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ප්‍රථම ජවන වශයෙන් උපදිනා කාම ජවන 29, ආවර්ජනද්වය ය, විපාක සිත් 36 චෛතසික 52, සියුලු රූප </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> පච්ඡාජාත ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>වස්තු  පුරෙජාත ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>වසත්වාරම්මණ  පුරෙජාත ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>ආරම්මණ පුරෙජාත ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>අරූප විපාක වර්ජිත ප්‍රථම භවංග ආදී පශ්විම පශ්විම වූ සිත් 85, චෛතසික 52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ප්‍රතිසන්ධිආදී පූර්ව පූර්ව චිත්තයන් හා ඉපද රූපස්ථිතියට පැමිණියා වූ ඒකජකය, ද්විජාකය, තිජකාය, චතුජකාය </t>
+  </si>
+  <si>
+    <t>සිත් 89, චෛතසික 52, පශ්විම පශ්විම චිත්තයන් හා උපදනා චිත්තජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඥ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප</t>
+  </si>
+  <si>
+    <t>සහජාතාස්ති  ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>වස්තු පුරේජාතාස්ති ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>වස්ත්වාරම්මණ පුරේජාතාස්ති ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>ආරම්මණ  පුරේජාතාස්ති ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">යම් කිසි ධර්මයක් ගරු කොට අරමුණු නො කරන අවස්ථාවෙහි වූ ද යම් කිසි ධර්මයක් අරමුණු නො කරන්නා වූ ලෞකික සිත් </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>81</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Iskoola Pota"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, එහි චෛතසික </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>52</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Iskoola Pota"/>
+        <family val="2"/>
+      </rPr>
+      <t>, චිත්තජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඥ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප (රූප සියල්ල)</t>
+    </r>
+  </si>
+  <si>
+    <t>යම් කිසි ධර්මයක් ගරු කොට අරමුණු නො කරන අවස්ථාවෙහි වූ ද යම් කිසි ධර්මයක් අරමුණු නො කරන්නා වූ ලෞකික සිත් 81, එහි චෛතසික 52, චිත්තජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඥ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප (රූප සියල්ල)</t>
+  </si>
+  <si>
+    <r>
+      <t>දේහේතුක, තිහේතුවක ජවන් සිත් 52</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
         <color rgb="FF231F20"/>
-        <rFont val="Iskoola Pota"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> සිත්</t>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
     </r>
     <r>
       <rPr>
@@ -1242,270 +1615,75 @@
         <color rgb="FF231F20"/>
         <rFont val="FMAbhaya"/>
       </rPr>
-      <t xml:space="preserve"> 52" Pkao úÑlsÉPd yer ffp;isl mKi h" idêm;s Ñ;a;c rEm</t>
-    </r>
-  </si>
-  <si>
-    <t>චිත්තජ රූප, හාර්දය වස්තුවෙන් අන්‍ය වූ ප්‍රතිසන්ධී කර්මජ රූප, සකල උපාදාය රූප</t>
-  </si>
-  <si>
-    <t>නැත</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">සිත් 89, චෛතසික </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
+      <t xml:space="preserve"> විචිකිච්ඡා   වර්ජිත චෛතසික 51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF231F20"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t>52</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Iskoola Pota"/>
-        <family val="2"/>
-      </rPr>
-      <t>,  සකල මහා භූතයෝ, ප්‍රතිසන්ධි වස්තු රූප</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">සිත් 89, චෛතසික </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>52</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>සිත් 89</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t>,</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Iskoola Pota"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> චෛතසික 5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Iskoola Pota"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, රූප </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>28</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Iskoola Pota"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, නිර්වාණය, ප්‍රඥප්තින් </t>
-    </r>
-  </si>
-  <si>
-    <t>සහාජාත අධිපති ප්‍රත්‍යය නොලබන්නාවූද, සහාජාත අධිපති ප්‍රත්‍යය නොලබන්න අවස්ථාවේ වූද කාමාවචර සිත් 54, මහග්ගත විපාක සිත් 9, එහි යෙදන චෛතසික 52, ඒ ඒ  අවස්ථාව අධිපති ප්‍රත්‍යවන ධර්ම,  නිරාධිපති චිත්තජ රූප, ප්‍රතිසන්ධී කර්මජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඥ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">කිසි ධර්මයක් අරමුණු නො කරන්නා වූ ලෞකික සිත් </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>81</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Iskoola Pota"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, එහි චෛතසික </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>52</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Iskoola Pota"/>
-        <family val="2"/>
-      </rPr>
-      <t>, චිත්තජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඥ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප (රූප සියල්ල)</t>
-    </r>
-  </si>
-  <si>
-    <t>සිත් 89 හි ඇති චේතනාව</t>
-  </si>
-  <si>
-    <t>අතීත වූ කුසල අකුසල චේතනා 33</t>
-  </si>
-  <si>
-    <t>විපාක ප්‍රත්‍යය</t>
-  </si>
-  <si>
-    <t>විපාක සිත් 36, චෛතසික 38, යන ප්‍රවුර්ත්ති ප්‍රතිසන්ධි නාමස්කන්ධ</t>
-  </si>
-  <si>
-    <t>නාම ආහාර ප්‍රත්‍යය</t>
-  </si>
-  <si>
-    <t>රූප ආහාර ප්‍රත්‍යය (උපත්ථමභකත්වය)</t>
-  </si>
-  <si>
-    <t>රූප ආහාර ප්‍රත්‍යය (ජනකත්වය)</t>
-  </si>
-  <si>
-    <t>ඔවුනොවුන්ට හා චිත්තජ රූප ප්‍රතිසන්ධි කර්මජ රුපයන්ට ද ප්‍රත්‍යය ව සිත් 89, චෛතසික 52 යන ප්‍රතිසන්ධි නාමස්කන්ධ,ඔවුනොවුන්ට හා උපාදාය රුපයන්ට ප්‍රත්‍යය වන චිත්තජ ප්‍රතිසන්ධි කර්මජ බාහිර අහාරාජ ඍතුජ අසංඥ සත්ව කර්මජ ප්‍රවුර්තික කර්මජ රූපයන්ට අයත් වූ සකල මහා භූතයෝ ය, පඤවවොකාර  ප්‍රතිසන්ධි නාමස්කන්ධයන්ට ප්‍රත්‍යය වන හර්දය වස්තුව ය, හර්දය වස්තුවට ප්‍රත්‍යය වන පඤවවොකාර ප්‍රතිසන්ධි නාමස්කන්ධ</t>
-  </si>
-  <si>
-    <t>ඔවුනොවුන්ගෙන් ප්‍රත්‍යය ලබන සිත් 89, චෛතසික 52, යන ප්‍රවුර්ත්ති ප්‍රතිසන්ධි නාමස්කන්ධ,  නාමස්කන්ධයන්ගෙන් ප්‍රත්‍යය ලබන චිත්තජ රූප හා ප්‍රතිසන්ධි කර්මජ රූප, ඔවුනොවුන්ගෙන් ප්‍රත්‍යය ලබන සකල මහා  භූතයෝ,  මහා භූතයන්ගෙන් ප්‍රත්‍යය ලබන උපදය රූප, හර්දයවස්තුවෙන් ප්‍රත්‍යය ලබන පඤවෝකාර  ප්‍රතිසන්ධි නාමස්කන්ධ, පඤවෝකාර ප්‍රතිසන්ධි නාමස්කන්ධයන්ගෙන් ප්‍රත්‍යය ලබන හර්දය වස්තුව</t>
-  </si>
-  <si>
-    <t>චිත්තජ රූප, ප්‍රතිසන්ධී කර්මජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඤ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප (රූප සියල්ල)</t>
-  </si>
-  <si>
-    <t>චිත්තජ රූප, ප්‍රතිසන්ධී කර්මජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඤ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප</t>
-  </si>
-  <si>
-    <t>අවිගත ප්‍රත්‍යය</t>
-  </si>
-  <si>
-    <t>විගත ප්‍රත්‍යය</t>
-  </si>
-  <si>
-    <t>නාස්ති  ප්‍රත්‍යය</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">අහේතුක සිත් </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>18,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Iskoola Pota"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ඡන්දය වර්ජිත අන්‍යසමාන චෛතසික </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>12</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Iskoola Pota"/>
-        <family val="2"/>
-      </rPr>
-      <t>, මෝහ මූල ද්විත්වයේ (සිත් දෙකේ) මෝහය, අහේතුක චිත්තජ රූප, අහේතුක ප්‍රතිසන්ධි කර්මජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඥ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප</t>
-    </r>
-  </si>
-  <si>
-    <t>සිත් 89, චේතනාව හැර චෛතසික 51, චිත්තජ රූප, ප්‍රතිසන්ධී කර්මජ රූප</t>
-  </si>
-  <si>
-    <t>සිත් 89හි ඇති චේතනා 89, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප, අසංඥ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප</t>
-  </si>
-  <si>
-    <t>විපාක සිත් 36, අහි ඇතුලත්  චෛතසික 38, චිත්තජ රූප, ප්‍රතිසන්ධී කර්මජ රූප,  අසංඥ සත්ව කර්මජ රූප, ප්‍රවෘත්ති කර්මජ රූප</t>
-  </si>
-  <si>
-    <t>වර්තමාන</t>
-  </si>
-  <si>
-    <t>කුසල් සිත් 21, අකුසල් සිත් 12, ක්‍රියා සිත් 20, චෛතසික 52, චිත්තජ රූප, බාහිර රූප, ආහාරජ රූප, ඍතුජ රූප</t>
-  </si>
-  <si>
-    <t>සම්පයුත්ත ප්‍රත්‍යය</t>
-  </si>
-  <si>
-    <t>විප්පයුත්ත ප්‍රත්‍යය</t>
-  </si>
-  <si>
-    <t>අස්ථි ප්‍රත්‍යයට සමානයි</t>
+        <color rgb="FF231F20"/>
+        <rFont val="FMAbhaya"/>
+      </rPr>
+      <t xml:space="preserve"> සාධිපති චිත්තජ රූප </t>
+    </r>
+  </si>
+  <si>
+    <t>සහාජාත ප්‍රත්‍යයට සමානයි</t>
+  </si>
+  <si>
+    <t>වස්තු පුරේජාත නිස්සය ප්‍රත්‍යයට සමානයි</t>
+  </si>
+  <si>
+    <t>වසත්වාරම්මණ  පුරෙජාත නිශ්‍රය ප්‍රත්‍යයට සමානයි</t>
+  </si>
+  <si>
+    <t>ආරම්මණ පුරෙජාත ප්‍රත්‍යයට සමානයි</t>
+  </si>
+  <si>
+    <t>පශ්චාජ්ජාතාසති ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>ආහාරාසති ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>ඉන්ද්‍රියාසති ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>පශ්වජ්ජාත ප්‍රත්‍යයට සමානයි</t>
+  </si>
+  <si>
+    <t>රූපාහාර ප්‍රත්‍යයට සමානයි</t>
+  </si>
+  <si>
+    <t>රූපජිවිතීත්ද්‍රියාසති ප්‍රත්‍යයට සමානයි</t>
+  </si>
+  <si>
+    <t>සහජාත විප්පයුත්ත ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>වස්තු පුරේජාත විප්පයුත්ත ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>වස්ත්වාරම්මණ පුරේජාත  විප්පයුත්ත ප්‍රත්‍යය</t>
+  </si>
+  <si>
+    <t>පශ්චාජ්ජාත විප්පයුත්ත ප්‍රත්‍යය</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1569,6 +1747,18 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="FMAbhaya"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF231F20"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1708,7 +1898,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1743,6 +1933,51 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1753,58 +1988,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2086,17 +2279,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:H46"/>
+  <dimension ref="B3:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C21"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="36.28515625" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" customWidth="1"/>
     <col min="7" max="7" width="50.85546875" customWidth="1"/>
@@ -2110,19 +2303,19 @@
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="27" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2133,73 +2326,75 @@
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
     </row>
     <row r="7" spans="2:8" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="15"/>
-      <c r="C7" s="25" t="s">
+      <c r="B7" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" s="15"/>
+      <c r="G7" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="25"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="16"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="21"/>
-      <c r="C9" s="27" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="22" t="s">
+      <c r="E9" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="21"/>
+      <c r="G9" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="2:8" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8"/>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -2209,88 +2404,88 @@
         <v>62</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:8" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="32" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="32" t="s">
-        <v>70</v>
+      <c r="G11" s="18" t="s">
+        <v>116</v>
       </c>
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="2:8" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="31" t="s">
+      <c r="D12" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="2:8" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="31" t="s">
+      <c r="D13" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="31" t="s">
+      <c r="F13" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="2:8" ht="221.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="15" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>3</v>
+        <v>96</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H14" s="9"/>
     </row>
@@ -2298,7 +2493,7 @@
       <c r="B15" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -2308,44 +2503,50 @@
         <v>53</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="221.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="20" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="G16" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H16" s="9"/>
     </row>
     <row r="17" spans="2:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="8"/>
-      <c r="C17" s="28"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="7" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="9"/>
+      <c r="F17" s="19" t="s">
+        <v>98</v>
+      </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="2:8" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="8"/>
-      <c r="C18" s="26"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="7" t="s">
         <v>33</v>
       </c>
@@ -2356,386 +2557,550 @@
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="2:8" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8"/>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+        <v>89</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>117</v>
+      </c>
       <c r="H19" s="9"/>
     </row>
-    <row r="20" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="8"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="8"/>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="8"/>
-      <c r="C23" s="24" t="s">
-        <v>37</v>
-      </c>
+      <c r="C23" s="21"/>
       <c r="D23" s="7" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="8"/>
-      <c r="C24" s="24" t="s">
-        <v>38</v>
-      </c>
+      <c r="C24" s="22"/>
       <c r="D24" s="7" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" s="19" t="s">
+    <row r="25" spans="2:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="8"/>
+      <c r="C25" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="8"/>
+      <c r="C26" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E27" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="2:8" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="31"/>
+      <c r="D28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="8"/>
+      <c r="C29" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F25" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="2:8" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="8"/>
-      <c r="C27" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="8"/>
-      <c r="C28" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="2:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="8"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
     </row>
-    <row r="30" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="8"/>
-      <c r="C30" s="26"/>
+      <c r="C30" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="D30" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
     </row>
-    <row r="31" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="8"/>
-      <c r="C31" s="25" t="s">
-        <v>44</v>
-      </c>
+      <c r="C31" s="21"/>
       <c r="D31" s="7" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
     </row>
-    <row r="32" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="8"/>
-      <c r="C32" s="28"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="7" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
     </row>
-    <row r="33" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="8"/>
-      <c r="C33" s="26"/>
+      <c r="C33" s="20" t="s">
+        <v>44</v>
+      </c>
       <c r="D33" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
     </row>
-    <row r="34" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="8"/>
-      <c r="C34" s="24" t="s">
-        <v>45</v>
-      </c>
+      <c r="C34" s="21"/>
       <c r="D34" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>57</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
     </row>
-    <row r="35" spans="2:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="8"/>
-      <c r="C35" s="24" t="s">
-        <v>46</v>
-      </c>
+      <c r="C35" s="22"/>
       <c r="D35" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>56</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E35" s="9"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
     </row>
-    <row r="36" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="8"/>
-      <c r="C36" s="24" t="s">
-        <v>47</v>
+      <c r="C36" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" s="9"/>
+        <v>54</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
     </row>
-    <row r="37" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="8"/>
-      <c r="C37" s="24" t="s">
-        <v>48</v>
+      <c r="C37" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E37" s="9"/>
+        <v>55</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
     </row>
-    <row r="38" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="8"/>
-      <c r="C38" s="25" t="s">
-        <v>49</v>
+      <c r="C38" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
     </row>
-    <row r="39" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="8"/>
-      <c r="C39" s="28"/>
+      <c r="C39" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="D39" s="7" t="s">
-        <v>3</v>
+        <v>129</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
     </row>
-    <row r="40" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="8"/>
-      <c r="C40" s="28"/>
+      <c r="C40" s="21"/>
       <c r="D40" s="7" t="s">
-        <v>3</v>
+        <v>130</v>
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
     </row>
-    <row r="41" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="8"/>
-      <c r="C41" s="26"/>
+      <c r="C41" s="21"/>
       <c r="D41" s="7" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
     </row>
-    <row r="42" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="8"/>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="22"/>
+      <c r="D42" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+    </row>
+    <row r="43" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="8"/>
+      <c r="C43" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H43" s="9"/>
+    </row>
+    <row r="44" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="8"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="H44" s="9"/>
+    </row>
+    <row r="45" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="8"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H45" s="9"/>
+    </row>
+    <row r="46" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="8"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H46" s="9"/>
+    </row>
+    <row r="47" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="8"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H47" s="9"/>
+    </row>
+    <row r="48" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="8"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H48" s="9"/>
+    </row>
+    <row r="49" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="8"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H49" s="9"/>
+    </row>
+    <row r="50" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="8"/>
+      <c r="C50" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E42" s="31" t="s">
+      <c r="D50" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F42" s="31" t="s">
+      <c r="F50" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G42" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="H42" s="9"/>
-    </row>
-    <row r="43" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="8"/>
-      <c r="C43" s="24" t="s">
+      <c r="G50" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H50" s="9"/>
+    </row>
+    <row r="51" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="8"/>
+      <c r="C51" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E43" s="31" t="s">
+      <c r="D51" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E51" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F43" s="31" t="s">
+      <c r="F51" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G43" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="H43" s="9"/>
-    </row>
-    <row r="44" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="8"/>
-      <c r="C44" s="24" t="s">
+      <c r="G51" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H51" s="9"/>
+    </row>
+    <row r="52" spans="2:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="8"/>
+      <c r="C52" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H44" s="9"/>
-    </row>
-    <row r="45" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="8"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-    </row>
-    <row r="46" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="8"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
+      <c r="D52" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H52" s="9"/>
+    </row>
+    <row r="53" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="8"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+    </row>
+    <row r="54" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="8"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C38:C41"/>
+  <mergeCells count="21">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="C43:C49"/>
     <mergeCell ref="C19:C21"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
@@ -2744,11 +3109,13 @@
     <mergeCell ref="F4:F6"/>
     <mergeCell ref="G4:G6"/>
     <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C39:C42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>